<commit_message>
se agregaron checks y defaults a la base de datos
</commit_message>
<xml_diff>
--- a/Documentacion del Proyecto/Diccionario de datos.xlsx
+++ b/Documentacion del Proyecto/Diccionario de datos.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PROGRAMACION INA\PAE Java\Proyecto_Paew_Sistema_de_Facturaci-n\Documentacion del Proyecto\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PROGRAMACION INA\PAE Java\PROYECTO_PAE_FACTURACION\Documentacion del Proyecto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A34BDE36-F5CB-4C21-87DC-0355587002E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88D0E133-CE6B-4F50-9FA0-126ACF85467B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25080" yWindow="300" windowWidth="19440" windowHeight="15600" xr2:uid="{D39DC26D-940D-4750-96A8-DB1A6D2D162E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15990" xr2:uid="{D39DC26D-940D-4750-96A8-DB1A6D2D162E}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="54">
   <si>
     <t>Tabla: CLIENTES</t>
   </si>
@@ -53,9 +53,6 @@
     <t>Restricción</t>
   </si>
   <si>
-    <t>Null</t>
-  </si>
-  <si>
     <t>Otras</t>
   </si>
   <si>
@@ -180,6 +177,27 @@
   </si>
   <si>
     <t>PRECIO_UNITARIO</t>
+  </si>
+  <si>
+    <t>Not Null</t>
+  </si>
+  <si>
+    <t>SI</t>
+  </si>
+  <si>
+    <t>CHECK (&gt;= 0)</t>
+  </si>
+  <si>
+    <t>UNIQUE</t>
+  </si>
+  <si>
+    <t>DEFAULT GETDATE()</t>
+  </si>
+  <si>
+    <t>DEFAULT 'Efectivo'</t>
+  </si>
+  <si>
+    <t>CHECK('Simpe', 'Efectivo', 'Tarjeta')</t>
   </si>
 </sst>
 </file>
@@ -692,15 +710,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E91AAB2-37B0-4C89-949A-C9559734E26B}">
   <dimension ref="A1:F73"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A67" activeCellId="6" sqref="A4:F4 A13:F13 A23:F23 A34:F34 A46:F46 A57:F57 A67:F67"/>
+    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="G39" sqref="G39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22.7109375" customWidth="1"/>
     <col min="2" max="2" width="14.42578125" customWidth="1"/>
-    <col min="6" max="6" width="15.5703125" customWidth="1"/>
+    <col min="4" max="4" width="19" customWidth="1"/>
+    <col min="6" max="6" width="31.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -723,52 +742,59 @@
         <v>4</v>
       </c>
       <c r="E4" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="F4" s="4" t="s">
         <v>5</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B5" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="9" t="s">
         <v>8</v>
-      </c>
-      <c r="C5" s="9" t="s">
-        <v>9</v>
       </c>
       <c r="D5" s="9"/>
       <c r="E5" s="9"/>
       <c r="F5" s="10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" t="s">
         <v>11</v>
       </c>
-      <c r="B6" t="s">
-        <v>12</v>
+      <c r="E6" t="s">
+        <v>48</v>
       </c>
       <c r="F6" s="12"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="3" t="s">
         <v>13</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>14</v>
       </c>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="14"/>
+      <c r="E7" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="F7" s="14" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B10" s="2"/>
     </row>
@@ -786,61 +812,71 @@
         <v>4</v>
       </c>
       <c r="E13" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="F13" s="4" t="s">
         <v>5</v>
-      </c>
-      <c r="F13" s="4" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B14" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14" s="9" t="s">
         <v>8</v>
-      </c>
-      <c r="C14" s="9" t="s">
-        <v>9</v>
       </c>
       <c r="D14" s="9"/>
       <c r="E14" s="9"/>
       <c r="F14" s="10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B15" t="s">
         <v>11</v>
       </c>
-      <c r="B15" t="s">
-        <v>12</v>
+      <c r="E15" t="s">
+        <v>48</v>
       </c>
       <c r="F15" s="12"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B16" t="s">
         <v>13</v>
       </c>
-      <c r="B16" t="s">
-        <v>14</v>
-      </c>
-      <c r="F16" s="12"/>
+      <c r="E16" t="s">
+        <v>48</v>
+      </c>
+      <c r="F16" s="12" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="13" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
+      <c r="E17" s="3" t="s">
+        <v>48</v>
+      </c>
       <c r="F17" s="14"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="15" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B20" s="15"/>
     </row>
@@ -858,70 +894,86 @@
         <v>4</v>
       </c>
       <c r="E23" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="F23" s="4" t="s">
         <v>5</v>
-      </c>
-      <c r="F23" s="4" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B24" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C24" s="9" t="s">
         <v>8</v>
-      </c>
-      <c r="C24" s="9" t="s">
-        <v>9</v>
       </c>
       <c r="D24" s="9"/>
       <c r="E24" s="9"/>
       <c r="F24" s="10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B25" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="E25" t="s">
+        <v>48</v>
       </c>
       <c r="F25" s="12"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B26" t="s">
         <v>21</v>
       </c>
-      <c r="B26" t="s">
-        <v>22</v>
+      <c r="E26" t="s">
+        <v>48</v>
       </c>
       <c r="F26" s="12"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="B27" t="s">
         <v>23</v>
       </c>
-      <c r="B27" t="s">
-        <v>24</v>
+      <c r="D27" t="s">
+        <v>49</v>
+      </c>
+      <c r="E27" t="s">
+        <v>48</v>
       </c>
       <c r="F27" s="12"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="13" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C28" s="3"/>
-      <c r="D28" s="3"/>
-      <c r="E28" s="3"/>
+      <c r="D28" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>48</v>
+      </c>
       <c r="F28" s="14"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B31" s="2"/>
     </row>
@@ -939,89 +991,101 @@
         <v>4</v>
       </c>
       <c r="E34" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="F34" s="4" t="s">
         <v>5</v>
-      </c>
-      <c r="F34" s="4" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B35" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C35" s="9" t="s">
         <v>8</v>
-      </c>
-      <c r="C35" s="9" t="s">
-        <v>9</v>
       </c>
       <c r="D35" s="9"/>
       <c r="E35" s="9"/>
       <c r="F35" s="10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="B36" t="s">
         <v>28</v>
       </c>
-      <c r="B36" t="s">
-        <v>29</v>
-      </c>
-      <c r="F36" s="12"/>
+      <c r="D36" t="s">
+        <v>52</v>
+      </c>
+      <c r="F36" s="12" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="B37" t="s">
         <v>30</v>
       </c>
-      <c r="B37" t="s">
-        <v>31</v>
+      <c r="D37" t="s">
+        <v>51</v>
       </c>
       <c r="F37" s="12"/>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B38" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C38" t="s">
+        <v>31</v>
+      </c>
+      <c r="F38" s="12" t="s">
         <v>32</v>
-      </c>
-      <c r="F38" s="12" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B39" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C39" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F39" s="12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C40" s="3"/>
-      <c r="D40" s="3"/>
-      <c r="E40" s="3"/>
+      <c r="D40" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="E40" s="3" t="s">
+        <v>48</v>
+      </c>
       <c r="F40" s="14"/>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B43" s="2"/>
     </row>
@@ -1039,80 +1103,90 @@
         <v>4</v>
       </c>
       <c r="E46" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="F46" s="4" t="s">
         <v>5</v>
-      </c>
-      <c r="F46" s="4" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B47" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C47" s="9" t="s">
         <v>8</v>
-      </c>
-      <c r="C47" s="9" t="s">
-        <v>9</v>
       </c>
       <c r="D47" s="9"/>
       <c r="E47" s="9"/>
       <c r="F47" s="10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B48" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C48" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F48" s="12" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B49" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C49" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F49" s="12" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B50" t="s">
-        <v>8</v>
+        <v>7</v>
+      </c>
+      <c r="D50" t="s">
+        <v>49</v>
+      </c>
+      <c r="E50" t="s">
+        <v>48</v>
       </c>
       <c r="F50" s="12"/>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="13" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C51" s="3"/>
-      <c r="D51" s="3"/>
-      <c r="E51" s="3"/>
+      <c r="D51" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="E51" s="3" t="s">
+        <v>48</v>
+      </c>
       <c r="F51" s="14"/>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B54" s="2"/>
     </row>
@@ -1130,61 +1204,71 @@
         <v>4</v>
       </c>
       <c r="E57" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="F57" s="7" t="s">
         <v>5</v>
-      </c>
-      <c r="F57" s="7" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" s="8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B58" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C58" s="9" t="s">
         <v>8</v>
-      </c>
-      <c r="C58" s="9" t="s">
-        <v>9</v>
       </c>
       <c r="D58" s="9"/>
       <c r="E58" s="9"/>
       <c r="F58" s="10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="B59" t="s">
         <v>30</v>
       </c>
-      <c r="B59" t="s">
-        <v>31</v>
+      <c r="D59" t="s">
+        <v>51</v>
       </c>
       <c r="F59" s="12"/>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" s="11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B60" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="E60" t="s">
+        <v>48</v>
       </c>
       <c r="F60" s="12"/>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" s="13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C61" s="3"/>
-      <c r="D61" s="3"/>
-      <c r="E61" s="3"/>
+      <c r="D61" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="E61" s="3" t="s">
+        <v>48</v>
+      </c>
       <c r="F61" s="14"/>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B64" s="2"/>
     </row>
@@ -1202,84 +1286,100 @@
         <v>4</v>
       </c>
       <c r="E67" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="F67" s="4" t="s">
         <v>5</v>
-      </c>
-      <c r="F67" s="4" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B68" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C68" s="9" t="s">
         <v>8</v>
-      </c>
-      <c r="C68" s="9" t="s">
-        <v>9</v>
       </c>
       <c r="D68" s="9"/>
       <c r="E68" s="9"/>
       <c r="F68" s="10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" s="11" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B69" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C69" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F69" s="12" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" s="11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B70" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C70" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F70" s="12" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" s="11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B71" t="s">
-        <v>8</v>
+        <v>7</v>
+      </c>
+      <c r="D71" t="s">
+        <v>49</v>
+      </c>
+      <c r="E71" t="s">
+        <v>48</v>
       </c>
       <c r="F71" s="12"/>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" s="11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B72" t="s">
-        <v>24</v>
+        <v>23</v>
+      </c>
+      <c r="D72" t="s">
+        <v>49</v>
+      </c>
+      <c r="E72" t="s">
+        <v>48</v>
       </c>
       <c r="F72" s="12"/>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" s="13" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C73" s="3"/>
-      <c r="D73" s="3"/>
-      <c r="E73" s="3"/>
+      <c r="D73" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="E73" s="3" t="s">
+        <v>48</v>
+      </c>
       <c r="F73" s="14"/>
     </row>
   </sheetData>

</xml_diff>